<commit_message>
Added LOINC codes for MMC. Created stub HearingObservation.
</commit_message>
<xml_diff>
--- a/output/CodeSystem-SPLASCHMultiModalCommunicationObservationCS.xlsx
+++ b/output/CodeSystem-SPLASCHMultiModalCommunicationObservationCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-14T15:55:03-04:00</t>
+    <t>2022-03-24T15:01:17-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -123,7 +123,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>7</t>
+    <t>1</t>
   </si>
   <si>
     <t>Level</t>
@@ -136,63 +136,6 @@
   </si>
   <si>
     <t>Definition</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>convey-simple-messages-low-demand</t>
-  </si>
-  <si>
-    <t>Convey simple meaningful messages in low demand situations</t>
-  </si>
-  <si>
-    <t>How often does the individual convey simple messages that are meaningful related to routine daily activities in LOW demand situations (e.g., request actions, request objects, initiate greetings)?</t>
-  </si>
-  <si>
-    <t>short-conversations-low-demand</t>
-  </si>
-  <si>
-    <t>Participate in short structured conversations in low demand situations</t>
-  </si>
-  <si>
-    <t>How often does the individual participate in short structured conversations that are meaningful in LOW demand situations (e.g., familiar and predictable conversations, sharing opinions, expressing like or dislike about the immediate environment)?</t>
-  </si>
-  <si>
-    <t>convey-complex-messages-low-demand</t>
-  </si>
-  <si>
-    <t>Convey complex messages in low demand situations</t>
-  </si>
-  <si>
-    <t>How often does the individual convey complex messages that are meaningful in LOW demand situations (e.g., telling a story, discussion school/current events, describing things outside the immediate environment)?</t>
-  </si>
-  <si>
-    <t>convey-simple-messages-high-demand</t>
-  </si>
-  <si>
-    <t>Convey simple meaningful messages in high demand situations</t>
-  </si>
-  <si>
-    <t>How often does the individual convey simple messages that are meaningful related to routine daily activities in HIGH demand situations (e.g., request actions, request objects, initiate greetings)?</t>
-  </si>
-  <si>
-    <t>short-conversations-high-demand</t>
-  </si>
-  <si>
-    <t>Participate in short structured conversations in high demand situations</t>
-  </si>
-  <si>
-    <t>How often does the individual participate in short structured conversations that are meaningful in HIGH demand situations (e.g., familiar and predictable conversations, sharing opinions, expressing like or dislike about the immediate environment)?</t>
-  </si>
-  <si>
-    <t>convey-complex-messages-high-demand</t>
-  </si>
-  <si>
-    <t>Convey complex messages in high demand situations</t>
-  </si>
-  <si>
-    <t>How often does the individual convey complex messages that are meaningful in HIGH demand situations (e.g., telling a story, discussion school/current events, describing things outside the immediate environment)?</t>
   </si>
   <si>
     <t>communicate-without-assistance</t>
@@ -522,7 +465,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -544,100 +487,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="D2" t="s" s="2">
         <v>43</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix code systems and value sets for multi-modal communication
</commit_message>
<xml_diff>
--- a/output/CodeSystem-SPLASCHMultiModalCommunicationObservationCS.xlsx
+++ b/output/CodeSystem-SPLASCHMultiModalCommunicationObservationCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-29T14:17:18-04:00</t>
+    <t>2022-04-05T11:13:11-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -123,19 +123,64 @@
     <t>Count</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Display</t>
-  </si>
-  <si>
-    <t>Definition</t>
+    <t>99829-4</t>
+  </si>
+  <si>
+    <t>How often does the individual convey simple messages that are meaningful related to routine daily activities in LOW demand situations?</t>
+  </si>
+  <si>
+    <t>99830-2</t>
+  </si>
+  <si>
+    <t>How often does the individual participate in short structured conversations that are meaningful in LOW demand situations?</t>
+  </si>
+  <si>
+    <t>99831-0</t>
+  </si>
+  <si>
+    <t>How often does the individual convey complex messages that are meaningful in LOW demand situations?</t>
+  </si>
+  <si>
+    <t>99832-8</t>
+  </si>
+  <si>
+    <t>How often does the individual convey simple messages that are meaningful related to routine daily activities in HIGH demand situations?</t>
+  </si>
+  <si>
+    <t>99833-6</t>
+  </si>
+  <si>
+    <t>How often does the individual participate in short structured conversations that are meaningful in HIGH demand situations?</t>
+  </si>
+  <si>
+    <t>99834-4</t>
+  </si>
+  <si>
+    <t>How often does the individual convey complex messages that are meaningful in HIGH demand situations?</t>
+  </si>
+  <si>
+    <t>99835-1</t>
+  </si>
+  <si>
+    <t>Functional Communication Measure - Multi-Modal Functional Communication score [ASHA NOMS]</t>
   </si>
   <si>
     <t>communicate-without-assistance</t>
@@ -465,7 +510,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -487,16 +532,100 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s" s="2">
         <v>43</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>